<commit_message>
added decision in adtjira IB, team config regresion cases
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/DataLoader/GenericUploader/ADTJira/Excel/Epic.xlsx
+++ b/src/test/resources/testdata/DataLoader/GenericUploader/ADTJira/Excel/Epic.xlsx
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1400" uniqueCount="826">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1404" uniqueCount="828">
   <si>
     <t>Title</t>
   </si>
@@ -2553,6 +2553,12 @@
   </si>
   <si>
     <t>2021-05-27T13:03:51Z</t>
+  </si>
+  <si>
+    <t>BOM-77667</t>
+  </si>
+  <si>
+    <t>2021-08-13T05:32:23Z</t>
   </si>
 </sst>
 </file>
@@ -9669,7 +9675,7 @@
     </row>
     <row r="2" spans="1:54" x14ac:dyDescent="0.3">
       <c r="A2" s="29" t="s">
-        <v>819</v>
+        <v>826</v>
       </c>
       <c r="B2" s="29"/>
       <c r="C2" s="29" t="s">
@@ -9687,7 +9693,7 @@
       <c r="K2" s="31"/>
       <c r="L2" s="28"/>
       <c r="M2" s="28" t="s">
-        <v>825</v>
+        <v>827</v>
       </c>
       <c r="N2" s="30"/>
       <c r="O2" s="28"/>

</xml_diff>